<commit_message>
Adição de novas classes para Modelos LAKEPORT e BAYSIDE
</commit_message>
<xml_diff>
--- a/WebServerSFC/TableErrorCodeROKU/ErrorCode.xlsx
+++ b/WebServerSFC/TableErrorCodeROKU/ErrorCode.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20616" windowHeight="11640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20616" windowHeight="11640" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="PT" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="RC" sheetId="3" r:id="rId3"/>
     <sheet name="LASER" sheetId="4" r:id="rId4"/>
     <sheet name="AUTO_OBA" sheetId="5" r:id="rId5"/>
+    <sheet name="CAL" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="89">
   <si>
     <t>FC01</t>
   </si>
@@ -636,7 +637,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -646,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1221,4 +1222,142 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="31.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>